<commit_message>
Change date format from yyyymmddhhmmss to %Y%m%d%H%M%S
</commit_message>
<xml_diff>
--- a/resources/CDAVariables_short.xlsx
+++ b/resources/CDAVariables_short.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="343">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmmss;start_date=20210101;end_date=20240730</t>
+    <t xml:space="preserve">date_format=%Y%m%d%H%M%S;start_date=20210101;end_date=20240730</t>
   </si>
   <si>
     <t xml:space="preserve">Set Identifier</t>
@@ -184,7 +184,35 @@
     <t xml:space="preserve">birth_date_ts</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmdd;start_date=19200101;end_date=20200730</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;start_date=19200101;end_date=20200730</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Author: creation date </t>
@@ -196,6 +224,37 @@
     <t xml:space="preserve">author_ts</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d%H%M%S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;start_date=20210101;end_date=20240730</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Author: prefix</t>
   </si>
   <si>
@@ -328,7 +387,25 @@
     <t xml:space="preserve">discharge_ts</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmmss</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d%H%M%S</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Time: begin of doctor contact</t>
@@ -442,7 +519,35 @@
     <t xml:space="preserve">complaint_start</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmdd;start_date=20210101;end_date=20240730</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;start_date=20210101;end_date=20240730</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Symptoms: duration</t>
@@ -496,7 +601,25 @@
     <t xml:space="preserve">triage_ts_start</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmm</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d%H%M</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Triage: end </t>
@@ -598,7 +721,35 @@
     <t xml:space="preserve">diagnostics_ts</t>
   </si>
   <si>
-    <t xml:space="preserve">date_format=yyyymmddhhmm;start_date=20210101;end_date=20240730</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">date_format=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">%Y%m%d%H%M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;start_date=20210101;end_date=20240730</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Diagnostic: Chest X-Ray</t>
@@ -1055,7 +1206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1099,6 +1250,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -1172,7 +1329,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -1197,11 +1354,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1209,7 +1366,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1466,7 +1623,7 @@
   <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1773,7 +1930,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>13</v>
@@ -1784,19 +1941,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>13</v>
@@ -1807,19 +1964,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>13</v>
@@ -1830,13 +1987,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>31</v>
@@ -1853,13 +2010,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>25</v>
@@ -1876,19 +2033,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>13</v>
@@ -1899,19 +2056,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>13</v>
@@ -1922,19 +2079,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>13</v>
@@ -1945,19 +2102,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>13</v>
@@ -1968,13 +2125,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>42</v>
@@ -1988,19 +2145,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>13</v>
@@ -2011,13 +2168,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>42</v>
@@ -2031,25 +2188,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2057,19 +2214,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>13</v>
@@ -2080,19 +2237,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>13</v>
@@ -2103,19 +2260,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>13</v>
@@ -2126,19 +2283,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>13</v>
@@ -2149,25 +2306,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2175,19 +2332,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>13</v>
@@ -2198,25 +2355,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,26 +2381,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2251,13 +2408,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>42</v>
@@ -2271,13 +2428,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>42</v>
@@ -2291,25 +2448,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,25 +2474,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,25 +2500,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I38" s="5"/>
     </row>
@@ -2370,22 +2527,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,13 +2550,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>42</v>
@@ -2413,19 +2570,19 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>13</v>
@@ -2436,19 +2593,19 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>13</v>
@@ -2459,19 +2616,19 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>13</v>
@@ -2482,19 +2639,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>13</v>
@@ -2505,25 +2662,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,19 +2688,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>13</v>
@@ -2554,25 +2711,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2580,25 +2737,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,13 +2763,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>42</v>
@@ -2626,19 +2783,19 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>13</v>
@@ -2649,25 +2806,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,25 +2832,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="G52" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,25 +2858,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,25 +2884,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,25 +2910,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,25 +2936,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2805,25 +2962,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2831,25 +2988,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2857,25 +3014,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2883,25 +3040,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,25 +3066,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2935,25 +3092,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2961,25 +3118,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2987,25 +3144,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,25 +3170,25 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,25 +3196,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3065,19 +3222,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>13</v>
@@ -3088,19 +3245,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>13</v>
@@ -3111,19 +3268,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>13</v>
@@ -3134,19 +3291,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>13</v>
@@ -3157,19 +3314,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>13</v>
@@ -3180,19 +3337,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>13</v>
@@ -3203,19 +3360,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>13</v>
@@ -3226,25 +3383,25 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3252,25 +3409,25 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,25 +3435,25 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3304,25 +3461,25 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="G77" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3330,19 +3487,19 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>13</v>
@@ -3353,19 +3510,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>13</v>
@@ -3376,13 +3533,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>42</v>
@@ -3396,19 +3553,19 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>13</v>
@@ -3419,19 +3576,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>13</v>
@@ -3442,19 +3599,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>13</v>
@@ -3465,19 +3622,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>13</v>
@@ -3488,13 +3645,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>42</v>
@@ -3508,25 +3665,25 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3534,22 +3691,22 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3557,25 +3714,25 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3583,25 +3740,25 @@
         <v>85</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3609,22 +3766,22 @@
         <v>86</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3632,42 +3789,42 @@
         <v>87</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>13</v>
@@ -3675,19 +3832,19 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>13</v>
@@ -3695,19 +3852,19 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>13</v>
@@ -3715,42 +3872,42 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>13</v>
@@ -3758,19 +3915,19 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>13</v>

</xml_diff>